<commit_message>
Add machine list withuser, pass
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomz/git/enersys/course/workshop-day1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151A398D-C258-A446-ACD5-B3E5BA3B0A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B01E471-4D32-A646-99E4-792A709244FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14260" yWindow="-23900" windowWidth="25820" windowHeight="20560" xr2:uid="{71E8DC99-28E6-CB47-BA6A-614DB3112A0D}"/>
+    <workbookView xWindow="5580" yWindow="-27780" windowWidth="33860" windowHeight="21060" xr2:uid="{71E8DC99-28E6-CB47-BA6A-614DB3112A0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>group</t>
   </si>
@@ -54,6 +54,30 @@
   </si>
   <si>
     <t>192.168.201.5</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>private_key_loc</t>
+  </si>
+  <si>
+    <t>/home/vagrant/.private_key</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>vagrant</t>
+  </si>
+  <si>
+    <t>!vault |
+$ANSIBLE_VAULT;1.1;AES256
+39353462346561356565643563353361346331623761633932326535396336396334343934623131
+3762656136666637623935383763306430333735313664360a353032386265313737313662613661
+38396133613236646530376364623131313533316531653530333532346238376364313163646639
+3734363866316632320a643230373634353737623464663666396235343963656264323764623063
+3564</t>
   </si>
 </sst>
 </file>
@@ -95,8 +119,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,39 +438,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419F49B6-F1C8-8743-A7B6-D0643620EF7A}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="295" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="295" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="323" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>